<commit_message>
done mau cho excel
</commit_message>
<xml_diff>
--- a/source-code/net-core/host/Ord.Zero.HttpHost/wwwroot/template/excel/ListUser.xlsx
+++ b/source-code/net-core/host/Ord.Zero.HttpHost/wwwroot/template/excel/ListUser.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15216263-80D9-4F95-B27E-F05718B5D9F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BEF0D1-DFC8-4AA8-8385-B4CB10D7CA87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sản phẩm" sheetId="1" r:id="rId1"/>
@@ -221,7 +221,38 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -247,8 +278,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="1"/>
-      <tableStyleElement type="headerRow" dxfId="0"/>
+      <tableStyleElement type="wholeTable" dxfId="6"/>
+      <tableStyleElement type="headerRow" dxfId="5"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -529,7 +560,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1057,6 +1088,14 @@
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A1:G1"/>
   </mergeCells>
+  <conditionalFormatting sqref="G5">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"Hoạt động"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"Không hoạt động"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F152" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>0</formula1>

</xml_diff>